<commit_message>
complete violin plot function
</commit_message>
<xml_diff>
--- a/data/poas/poas21.xlsx
+++ b/data/poas/poas21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaime/Desktop/poas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C665515-2A3D-E244-8199-FC21E505CAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1552C50C-D120-6448-8B38-AA7590A5E938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="21100" tabRatio="772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5481" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5483" uniqueCount="180">
   <si>
     <t>AB</t>
   </si>
@@ -9825,7 +9825,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="D189" sqref="D189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20733,7 +20733,9 @@
       <c r="C172" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D172" s="12"/>
+      <c r="D172" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="E172" s="12" t="s">
         <v>22</v>
       </c>
@@ -21802,6 +21804,9 @@
       </c>
       <c r="C189" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>22</v>
@@ -40514,6 +40519,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Modified0 xmlns="4233fc49-3339-4531-8895-cee7bd229291" xsi:nil="true"/>
+    <Priority xmlns="4233fc49-3339-4531-8895-cee7bd229291" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4233fc49-3339-4531-8895-cee7bd229291">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c93905bf-b08c-430b-8630-76f4d352397a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E4DDA97709D05344805E34443243448B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9eeeb8ecc7e5384bf1028f09b4198e68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4233fc49-3339-4531-8895-cee7bd229291" xmlns:ns3="c93905bf-b08c-430b-8630-76f4d352397a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24c3c3abd9978446371d5fdb96159abb" ns2:_="" ns3:_="">
     <xsd:import namespace="4233fc49-3339-4531-8895-cee7bd229291"/>
@@ -40745,29 +40772,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A1286C2-D303-4CB0-988E-81FAB35D11B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Modified0 xmlns="4233fc49-3339-4531-8895-cee7bd229291" xsi:nil="true"/>
-    <Priority xmlns="4233fc49-3339-4531-8895-cee7bd229291" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4233fc49-3339-4531-8895-cee7bd229291">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c93905bf-b08c-430b-8630-76f4d352397a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B407060D-E707-4A24-875F-4E4C1B032515}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c93905bf-b08c-430b-8630-76f4d352397a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4233fc49-3339-4531-8895-cee7bd229291"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D891CB69-F5BA-4210-B9BF-2F4C2B80A6D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -40784,29 +40814,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A1286C2-D303-4CB0-988E-81FAB35D11B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B407060D-E707-4A24-875F-4E4C1B032515}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c93905bf-b08c-430b-8630-76f4d352397a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4233fc49-3339-4531-8895-cee7bd229291"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>